<commit_message>
1.4 Códigos a Excel
</commit_message>
<xml_diff>
--- a/Alimentos.xlsx
+++ b/Alimentos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Carlos/Desktop/Granja/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Natasha GO\Desktop\Granja\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EF0B107-167D-6441-A231-6620272D21AA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0672CAD-01BF-4E56-A4A4-70BAC2072224}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="18300" windowHeight="14240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="11640" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Alimento Gral Cerdo" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,18 @@
     <sheet name="Alimento Granja Cerdo" sheetId="3" r:id="rId3"/>
     <sheet name="Alimento Granja Huevo" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -700,16 +711,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N32"/>
+  <dimension ref="A1:O32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="41.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="11" width="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -753,7 +773,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
@@ -796,8 +816,12 @@
       <c r="N2">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O2">
+        <f>+F2-I2</f>
+        <v>7.7787770571708936</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
@@ -841,7 +865,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
@@ -885,7 +909,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
@@ -929,7 +953,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
@@ -973,7 +997,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>19</v>
       </c>
@@ -1017,7 +1041,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>20</v>
       </c>
@@ -1061,7 +1085,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>21</v>
       </c>
@@ -1105,7 +1129,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>22</v>
       </c>
@@ -1149,7 +1173,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>23</v>
       </c>
@@ -1193,7 +1217,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>24</v>
       </c>
@@ -1237,7 +1261,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>25</v>
       </c>
@@ -1281,7 +1305,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>26</v>
       </c>
@@ -1325,7 +1349,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>27</v>
       </c>
@@ -1369,7 +1393,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>28</v>
       </c>
@@ -1413,7 +1437,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>29</v>
       </c>
@@ -1457,7 +1481,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>30</v>
       </c>
@@ -1501,7 +1525,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>31</v>
       </c>
@@ -1545,7 +1569,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>32</v>
       </c>
@@ -1589,7 +1613,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>33</v>
       </c>
@@ -1633,7 +1657,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>34</v>
       </c>
@@ -1677,7 +1701,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>35</v>
       </c>
@@ -1721,7 +1745,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>36</v>
       </c>
@@ -1765,7 +1789,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>37</v>
       </c>
@@ -1809,7 +1833,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>38</v>
       </c>
@@ -1853,7 +1877,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>39</v>
       </c>
@@ -1897,7 +1921,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>40</v>
       </c>
@@ -1941,7 +1965,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>41</v>
       </c>
@@ -1985,7 +2009,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>42</v>
       </c>
@@ -2029,7 +2053,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>43</v>
       </c>
@@ -2073,7 +2097,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>44</v>
       </c>
@@ -2128,12 +2152,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -2177,7 +2201,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>48</v>
       </c>
@@ -2221,7 +2245,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>49</v>
       </c>
@@ -2265,7 +2289,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>50</v>
       </c>
@@ -2309,7 +2333,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>51</v>
       </c>
@@ -2353,7 +2377,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>52</v>
       </c>
@@ -2397,7 +2421,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>53</v>
       </c>
@@ -2441,7 +2465,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>54</v>
       </c>
@@ -2485,7 +2509,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>55</v>
       </c>
@@ -2529,7 +2553,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>56</v>
       </c>
@@ -2573,7 +2597,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>57</v>
       </c>
@@ -2617,7 +2641,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>58</v>
       </c>
@@ -2661,7 +2685,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>59</v>
       </c>
@@ -2705,7 +2729,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>60</v>
       </c>
@@ -2749,7 +2773,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>61</v>
       </c>
@@ -2793,7 +2817,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>62</v>
       </c>
@@ -2837,7 +2861,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>63</v>
       </c>
@@ -2872,7 +2896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>64</v>
       </c>
@@ -2916,7 +2940,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>65</v>
       </c>
@@ -2960,7 +2984,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>66</v>
       </c>
@@ -3004,7 +3028,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>67</v>
       </c>
@@ -3048,7 +3072,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>68</v>
       </c>
@@ -3092,7 +3116,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>69</v>
       </c>
@@ -3136,7 +3160,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>70</v>
       </c>
@@ -3180,7 +3204,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>71</v>
       </c>
@@ -3233,14 +3257,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I118"/>
   <sheetViews>
-    <sheetView topLeftCell="A95" workbookViewId="0"/>
+    <sheetView topLeftCell="A107" workbookViewId="0">
+      <selection sqref="A1:I118"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="41.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="9" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>73</v>
       </c>
@@ -3269,7 +3296,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>74</v>
       </c>
@@ -3298,7 +3325,7 @@
         <v>1.536941586721432</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="1" t="s">
         <v>15</v>
@@ -3325,7 +3352,7 @@
         <v>1.7319611545856879</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="1" t="s">
         <v>16</v>
@@ -3352,7 +3379,7 @@
         <v>1.600941129150244</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="1" t="s">
         <v>18</v>
@@ -3379,7 +3406,7 @@
         <v>5.9625117519173561</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="1" t="s">
         <v>19</v>
@@ -3406,7 +3433,7 @@
         <v>1.3464255899653279</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="1" t="s">
         <v>22</v>
@@ -3433,7 +3460,7 @@
         <v>3.973523485382827</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="1" t="s">
         <v>24</v>
@@ -3460,7 +3487,7 @@
         <v>1.581050713849607</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="1" t="s">
         <v>29</v>
@@ -3487,7 +3514,7 @@
         <v>1.536941586721432</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="1" t="s">
         <v>30</v>
@@ -3514,7 +3541,7 @@
         <v>1.581050713849607</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="1" t="s">
         <v>32</v>
@@ -3541,7 +3568,7 @@
         <v>1.7319611545856879</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="1" t="s">
         <v>33</v>
@@ -3568,7 +3595,7 @@
         <v>5.9625117519173561</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="1" t="s">
         <v>34</v>
@@ -3595,7 +3622,7 @@
         <v>1.426831608952871</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="1" t="s">
         <v>35</v>
@@ -3622,7 +3649,7 @@
         <v>1.600941129150244</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="1" t="s">
         <v>40</v>
@@ -3649,7 +3676,7 @@
         <v>3.973523485382827</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>75</v>
       </c>
@@ -3678,7 +3705,7 @@
         <v>30.09568803566637</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="1" t="s">
         <v>16</v>
@@ -3696,7 +3723,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="1" t="s">
         <v>18</v>
@@ -3723,7 +3750,7 @@
         <v>3.840537009053075</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="1" t="s">
         <v>19</v>
@@ -3750,7 +3777,7 @@
         <v>1.442913663660099</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="1" t="s">
         <v>29</v>
@@ -3777,7 +3804,7 @@
         <v>30.09568803566637</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="1" t="s">
         <v>33</v>
@@ -3804,7 +3831,7 @@
         <v>3.840537009053075</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="1" t="s">
         <v>34</v>
@@ -3831,7 +3858,7 @@
         <v>1.5548894514272711</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="1" t="s">
         <v>35</v>
@@ -3849,7 +3876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="1" t="s">
         <v>38</v>
@@ -3876,7 +3903,7 @@
         <v>113.7702362952045</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>76</v>
       </c>
@@ -3905,7 +3932,7 @@
         <v>22.640382780496392</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="1" t="s">
         <v>15</v>
@@ -3932,7 +3959,7 @@
         <v>3.851224840633074</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="1" t="s">
         <v>16</v>
@@ -3959,7 +3986,7 @@
         <v>1.807199436297823</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="1" t="s">
         <v>18</v>
@@ -3986,7 +4013,7 @@
         <v>5.8047459683930844</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="1" t="s">
         <v>19</v>
@@ -4013,7 +4040,7 @@
         <v>1.7718938577514329</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="1" t="s">
         <v>24</v>
@@ -4040,7 +4067,7 @@
         <v>1.6350689614778211</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="1" t="s">
         <v>29</v>
@@ -4067,7 +4094,7 @@
         <v>3.83009944173976</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="1" t="s">
         <v>30</v>
@@ -4094,7 +4121,7 @@
         <v>1.6350689614778211</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="1" t="s">
         <v>32</v>
@@ -4121,7 +4148,7 @@
         <v>3.9883759673760522</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="1" t="s">
         <v>33</v>
@@ -4148,7 +4175,7 @@
         <v>5.8047459683930844</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="1" t="s">
         <v>34</v>
@@ -4175,7 +4202,7 @@
         <v>1.7718938577514329</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="1" t="s">
         <v>35</v>
@@ -4202,7 +4229,7 @@
         <v>2.0066335173842038</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>77</v>
       </c>
@@ -4231,7 +4258,7 @@
         <v>29.698484809834991</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="1" t="s">
         <v>21</v>
@@ -4258,7 +4285,7 @@
         <v>29.698484809834991</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="1" t="s">
         <v>23</v>
@@ -4285,7 +4312,7 @@
         <v>29.698484809834991</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="1" t="s">
         <v>33</v>
@@ -4303,7 +4330,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="1" t="s">
         <v>36</v>
@@ -4330,7 +4357,7 @@
         <v>29.698484809834991</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="1" t="s">
         <v>39</v>
@@ -4357,7 +4384,7 @@
         <v>29.698484809834991</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
       <c r="B43" s="1" t="s">
         <v>41</v>
@@ -4384,7 +4411,7 @@
         <v>29.698484809834991</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>78</v>
       </c>
@@ -4404,7 +4431,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
       <c r="B45" s="1" t="s">
         <v>32</v>
@@ -4422,7 +4449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>79</v>
       </c>
@@ -4451,7 +4478,7 @@
         <v>6.272751382759397</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
       <c r="B47" s="1" t="s">
         <v>18</v>
@@ -4469,7 +4496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
       <c r="B48" s="1" t="s">
         <v>19</v>
@@ -4496,7 +4523,7 @@
         <v>28.451583626178682</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
       <c r="B49" s="1" t="s">
         <v>20</v>
@@ -4523,7 +4550,7 @@
         <v>1.384228187751245</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
       <c r="B50" s="1" t="s">
         <v>21</v>
@@ -4550,7 +4577,7 @@
         <v>2.6824318445894288</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
       <c r="B51" s="1" t="s">
         <v>23</v>
@@ -4577,7 +4604,7 @@
         <v>5.9574034439013852</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="2"/>
       <c r="B52" s="1" t="s">
         <v>31</v>
@@ -4604,7 +4631,7 @@
         <v>6.272751382759397</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="2"/>
       <c r="B53" s="1" t="s">
         <v>33</v>
@@ -4622,7 +4649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="2"/>
       <c r="B54" s="1" t="s">
         <v>34</v>
@@ -4649,7 +4676,7 @@
         <v>28.451583626178682</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="2"/>
       <c r="B55" s="1" t="s">
         <v>36</v>
@@ -4676,7 +4703,7 @@
         <v>1.264891696711463</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="2"/>
       <c r="B56" s="1" t="s">
         <v>37</v>
@@ -4703,7 +4730,7 @@
         <v>5.4667828094514874</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="2"/>
       <c r="B57" s="1" t="s">
         <v>39</v>
@@ -4730,7 +4757,7 @@
         <v>2.6824318445894288</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="2"/>
       <c r="B58" s="1" t="s">
         <v>41</v>
@@ -4757,7 +4784,7 @@
         <v>5.9574034439013852</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="2"/>
       <c r="B59" s="1" t="s">
         <v>43</v>
@@ -4784,7 +4811,7 @@
         <v>4.3751504422066896</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="2"/>
       <c r="B60" s="1" t="s">
         <v>44</v>
@@ -4802,7 +4829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>80</v>
       </c>
@@ -4831,7 +4858,7 @@
         <v>8.8919790196779047</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="2"/>
       <c r="B62" s="1" t="s">
         <v>19</v>
@@ -4858,7 +4885,7 @@
         <v>23.461683917504679</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="2"/>
       <c r="B63" s="1" t="s">
         <v>20</v>
@@ -4885,7 +4912,7 @@
         <v>1.274987070542533</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="2"/>
       <c r="B64" s="1" t="s">
         <v>21</v>
@@ -4912,7 +4939,7 @@
         <v>1.274987070542533</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="2"/>
       <c r="B65" s="1" t="s">
         <v>23</v>
@@ -4939,7 +4966,7 @@
         <v>3.221993726959647</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="2"/>
       <c r="B66" s="1" t="s">
         <v>31</v>
@@ -4966,7 +4993,7 @@
         <v>8.8919790196779047</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="2"/>
       <c r="B67" s="1" t="s">
         <v>34</v>
@@ -4993,7 +5020,7 @@
         <v>23.461683917504679</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="2"/>
       <c r="B68" s="1" t="s">
         <v>36</v>
@@ -5020,7 +5047,7 @@
         <v>1.274987070542533</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="2"/>
       <c r="B69" s="1" t="s">
         <v>37</v>
@@ -5047,7 +5074,7 @@
         <v>10.05129700230629</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="2"/>
       <c r="B70" s="1" t="s">
         <v>39</v>
@@ -5074,7 +5101,7 @@
         <v>1.274987070542533</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="2"/>
       <c r="B71" s="1" t="s">
         <v>41</v>
@@ -5101,7 +5128,7 @@
         <v>3.221993726959647</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="2"/>
       <c r="B72" s="1" t="s">
         <v>44</v>
@@ -5128,7 +5155,7 @@
         <v>13.11389761958444</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>81</v>
       </c>
@@ -5157,7 +5184,7 @@
         <v>1.7427534079707869</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="2"/>
       <c r="B74" s="1" t="s">
         <v>15</v>
@@ -5184,7 +5211,7 @@
         <v>1.9049164999995001</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="2"/>
       <c r="B75" s="1" t="s">
         <v>16</v>
@@ -5211,7 +5238,7 @@
         <v>1.8749600192933411</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="2"/>
       <c r="B76" s="1" t="s">
         <v>19</v>
@@ -5238,7 +5265,7 @@
         <v>4.9497474683058327</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="2"/>
       <c r="B77" s="1" t="s">
         <v>22</v>
@@ -5265,7 +5292,7 @@
         <v>110.84643349328751</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="2"/>
       <c r="B78" s="1" t="s">
         <v>24</v>
@@ -5292,7 +5319,7 @@
         <v>1.7928988612527621</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="2"/>
       <c r="B79" s="1" t="s">
         <v>26</v>
@@ -5319,7 +5346,7 @@
         <v>2.9268868558020249</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="2"/>
       <c r="B80" s="1" t="s">
         <v>27</v>
@@ -5346,7 +5373,7 @@
         <v>3.4302575219167828</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="2"/>
       <c r="B81" s="1" t="s">
         <v>28</v>
@@ -5373,7 +5400,7 @@
         <v>2.70801280154532</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="2"/>
       <c r="B82" s="1" t="s">
         <v>29</v>
@@ -5400,7 +5427,7 @@
         <v>2.1645316190175361</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="2"/>
       <c r="B83" s="1" t="s">
         <v>30</v>
@@ -5427,7 +5454,7 @@
         <v>1.7928988612527621</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" s="2"/>
       <c r="B84" s="1" t="s">
         <v>32</v>
@@ -5454,7 +5481,7 @@
         <v>2.0173477492535499</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="2"/>
       <c r="B85" s="1" t="s">
         <v>35</v>
@@ -5481,7 +5508,7 @@
         <v>1.9456751264535119</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="2"/>
       <c r="B86" s="1" t="s">
         <v>38</v>
@@ -5508,7 +5535,7 @@
         <v>4.9497474683058327</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="2"/>
       <c r="B87" s="1" t="s">
         <v>40</v>
@@ -5535,7 +5562,7 @@
         <v>110.84643349328751</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="2"/>
       <c r="B88" s="1" t="s">
         <v>42</v>
@@ -5562,7 +5589,7 @@
         <v>2.794552524023088</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>82</v>
       </c>
@@ -5591,7 +5618,7 @@
         <v>64.200125595533009</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" s="2"/>
       <c r="B90" s="1" t="s">
         <v>15</v>
@@ -5618,7 +5645,7 @@
         <v>10.568458151135751</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" s="2"/>
       <c r="B91" s="1" t="s">
         <v>16</v>
@@ -5645,7 +5672,7 @@
         <v>2.5706468268171552</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" s="2"/>
       <c r="B92" s="1" t="s">
         <v>17</v>
@@ -5672,7 +5699,7 @@
         <v>4.358898943540674</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" s="2"/>
       <c r="B93" s="1" t="s">
         <v>18</v>
@@ -5699,7 +5726,7 @@
         <v>109.00438543451379</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" s="2"/>
       <c r="B94" s="1" t="s">
         <v>19</v>
@@ -5726,7 +5753,7 @@
         <v>82.875337932504991</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" s="2"/>
       <c r="B95" s="1" t="s">
         <v>23</v>
@@ -5753,7 +5780,7 @@
         <v>4.6680670167857077</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" s="2"/>
       <c r="B96" s="1" t="s">
         <v>24</v>
@@ -5780,7 +5807,7 @@
         <v>113.3181686797893</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="2"/>
       <c r="B97" s="1" t="s">
         <v>29</v>
@@ -5807,7 +5834,7 @@
         <v>43.245507431911093</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="2"/>
       <c r="B98" s="1" t="s">
         <v>30</v>
@@ -5834,7 +5861,7 @@
         <v>9.0756623482158894</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="2"/>
       <c r="B99" s="1" t="s">
         <v>31</v>
@@ -5861,7 +5888,7 @@
         <v>4.358898943540674</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" s="2"/>
       <c r="B100" s="1" t="s">
         <v>32</v>
@@ -5888,7 +5915,7 @@
         <v>169.46238520686529</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" s="2"/>
       <c r="B101" s="1" t="s">
         <v>33</v>
@@ -5915,7 +5942,7 @@
         <v>99.734730578251842</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" s="2"/>
       <c r="B102" s="1" t="s">
         <v>34</v>
@@ -5942,7 +5969,7 @@
         <v>82.875337932504991</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" s="2"/>
       <c r="B103" s="1" t="s">
         <v>35</v>
@@ -5969,7 +5996,7 @@
         <v>2.5706468268171552</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" s="2"/>
       <c r="B104" s="1" t="s">
         <v>41</v>
@@ -5996,7 +6023,7 @@
         <v>4.6680670167857077</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
         <v>83</v>
       </c>
@@ -6016,7 +6043,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" s="2"/>
       <c r="B106" s="1" t="s">
         <v>18</v>
@@ -6043,7 +6070,7 @@
         <v>10.56724498943157</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" s="2"/>
       <c r="B107" s="1" t="s">
         <v>20</v>
@@ -6070,7 +6097,7 @@
         <v>2.2999955238534819</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" s="2"/>
       <c r="B108" s="1" t="s">
         <v>21</v>
@@ -6097,7 +6124,7 @@
         <v>2.8192895756824279</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" s="2"/>
       <c r="B109" s="1" t="s">
         <v>23</v>
@@ -6124,7 +6151,7 @@
         <v>20.41230072544306</v>
       </c>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" s="2"/>
       <c r="B110" s="1" t="s">
         <v>25</v>
@@ -6151,7 +6178,7 @@
         <v>22.715633383201091</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" s="2"/>
       <c r="B111" s="1" t="s">
         <v>31</v>
@@ -6178,7 +6205,7 @@
         <v>64.346717087975819</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" s="2"/>
       <c r="B112" s="1" t="s">
         <v>33</v>
@@ -6205,7 +6232,7 @@
         <v>10.56724498943157</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" s="2"/>
       <c r="B113" s="1" t="s">
         <v>36</v>
@@ -6232,7 +6259,7 @@
         <v>2.1824916670676449</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" s="2"/>
       <c r="B114" s="1" t="s">
         <v>37</v>
@@ -6259,7 +6286,7 @@
         <v>5.9871657607046291</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" s="2"/>
       <c r="B115" s="1" t="s">
         <v>39</v>
@@ -6286,7 +6313,7 @@
         <v>2.8192895756824279</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" s="2"/>
       <c r="B116" s="1" t="s">
         <v>41</v>
@@ -6313,7 +6340,7 @@
         <v>20.41230072544306</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" s="2"/>
       <c r="B117" s="1" t="s">
         <v>43</v>
@@ -6331,7 +6358,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" s="2"/>
       <c r="B118" s="1" t="s">
         <v>44</v>
@@ -6360,16 +6387,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A2:A15"/>
+    <mergeCell ref="A16:A24"/>
+    <mergeCell ref="A25:A36"/>
+    <mergeCell ref="A37:A43"/>
+    <mergeCell ref="A44:A45"/>
     <mergeCell ref="A46:A60"/>
     <mergeCell ref="A61:A72"/>
     <mergeCell ref="A73:A88"/>
     <mergeCell ref="A89:A104"/>
     <mergeCell ref="A105:A118"/>
-    <mergeCell ref="A2:A15"/>
-    <mergeCell ref="A16:A24"/>
-    <mergeCell ref="A25:A36"/>
-    <mergeCell ref="A37:A43"/>
-    <mergeCell ref="A44:A45"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6379,15 +6406,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I101"/>
   <sheetViews>
-    <sheetView topLeftCell="A86" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
+      <selection sqref="A1:I101"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39" bestFit="1" customWidth="1"/>
+    <col min="4" max="9" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>73</v>
       </c>
@@ -6416,7 +6446,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>84</v>
       </c>
@@ -6445,7 +6475,7 @@
         <v>7.3865186429702936</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="1" t="s">
         <v>52</v>
@@ -6472,7 +6502,7 @@
         <v>110.68500636906811</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="1" t="s">
         <v>55</v>
@@ -6499,7 +6529,7 @@
         <v>2.5385910352879688</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="1" t="s">
         <v>56</v>
@@ -6526,7 +6556,7 @@
         <v>137.93880395437549</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="1" t="s">
         <v>57</v>
@@ -6553,7 +6583,7 @@
         <v>61.645238134144513</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="1" t="s">
         <v>58</v>
@@ -6580,7 +6610,7 @@
         <v>3.5512126254437528</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="1" t="s">
         <v>59</v>
@@ -6607,7 +6637,7 @@
         <v>6.164414002968976</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="1" t="s">
         <v>62</v>
@@ -6634,7 +6664,7 @@
         <v>3.4874775984943609</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="1" t="s">
         <v>64</v>
@@ -6661,7 +6691,7 @@
         <v>226.64233938079619</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="1" t="s">
         <v>66</v>
@@ -6688,7 +6718,7 @@
         <v>170.46765397761411</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="1" t="s">
         <v>67</v>
@@ -6706,7 +6736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="1" t="s">
         <v>70</v>
@@ -6733,7 +6763,7 @@
         <v>5.7811224847746594</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>85</v>
       </c>
@@ -6762,7 +6792,7 @@
         <v>5.4771113579171766</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="1" t="s">
         <v>50</v>
@@ -6780,7 +6810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="1" t="s">
         <v>52</v>
@@ -6807,7 +6837,7 @@
         <v>140.60811033735109</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="1" t="s">
         <v>55</v>
@@ -6834,7 +6864,7 @@
         <v>64.467552764760057</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="1" t="s">
         <v>56</v>
@@ -6861,7 +6891,7 @@
         <v>54.493746623375337</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="1" t="s">
         <v>57</v>
@@ -6888,7 +6918,7 @@
         <v>68.822753712499974</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="1" t="s">
         <v>58</v>
@@ -6915,7 +6945,7 @@
         <v>2.493628243780901</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="1" t="s">
         <v>59</v>
@@ -6933,7 +6963,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="1" t="s">
         <v>62</v>
@@ -6960,7 +6990,7 @@
         <v>121.73704896583079</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="1" t="s">
         <v>63</v>
@@ -6978,7 +7008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="1" t="s">
         <v>64</v>
@@ -7005,7 +7035,7 @@
         <v>3.7606990231680522</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="1" t="s">
         <v>65</v>
@@ -7032,7 +7062,7 @@
         <v>113.5904055261536</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="1" t="s">
         <v>66</v>
@@ -7059,7 +7089,7 @@
         <v>218.25797913145229</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="1" t="s">
         <v>70</v>
@@ -7086,7 +7116,7 @@
         <v>3.7529681739847631</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>86</v>
       </c>
@@ -7115,7 +7145,7 @@
         <v>6.1336556820662649</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="1" t="s">
         <v>50</v>
@@ -7142,7 +7172,7 @@
         <v>3.6426955361697151</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="1" t="s">
         <v>51</v>
@@ -7169,7 +7199,7 @@
         <v>1.8246004128758351</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="1" t="s">
         <v>55</v>
@@ -7187,7 +7217,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="1" t="s">
         <v>56</v>
@@ -7214,7 +7244,7 @@
         <v>247.09728178728849</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="1" t="s">
         <v>57</v>
@@ -7241,7 +7271,7 @@
         <v>410.67992402843362</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="1" t="s">
         <v>58</v>
@@ -7268,7 +7298,7 @@
         <v>32.058800143902253</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="1" t="s">
         <v>59</v>
@@ -7286,7 +7316,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="1" t="s">
         <v>60</v>
@@ -7313,7 +7343,7 @@
         <v>474.46865017617341</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="1" t="s">
         <v>61</v>
@@ -7340,7 +7370,7 @@
         <v>1.689927766460998</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="1" t="s">
         <v>62</v>
@@ -7367,7 +7397,7 @@
         <v>148.2039577926754</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="1" t="s">
         <v>64</v>
@@ -7394,7 +7424,7 @@
         <v>11.26604675668486</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="1" t="s">
         <v>65</v>
@@ -7412,7 +7442,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="1" t="s">
         <v>66</v>
@@ -7439,7 +7469,7 @@
         <v>170.77317492137709</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="1" t="s">
         <v>69</v>
@@ -7466,7 +7496,7 @@
         <v>5.6568542494923806</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
       <c r="B43" s="1" t="s">
         <v>70</v>
@@ -7493,7 +7523,7 @@
         <v>5.1302873376660196</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
       <c r="B44" s="1" t="s">
         <v>71</v>
@@ -7511,7 +7541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>87</v>
       </c>
@@ -7540,7 +7570,7 @@
         <v>6.2414157501448164</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
       <c r="B46" s="1" t="s">
         <v>51</v>
@@ -7558,7 +7588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
       <c r="B47" s="1" t="s">
         <v>52</v>
@@ -7585,7 +7615,7 @@
         <v>146.96788364649399</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
       <c r="B48" s="1" t="s">
         <v>55</v>
@@ -7612,7 +7642,7 @@
         <v>132.81827955750441</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
       <c r="B49" s="1" t="s">
         <v>56</v>
@@ -7639,7 +7669,7 @@
         <v>393.1805140983804</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
       <c r="B50" s="1" t="s">
         <v>57</v>
@@ -7666,7 +7696,7 @@
         <v>118.9014031541018</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
       <c r="B51" s="1" t="s">
         <v>58</v>
@@ -7693,7 +7723,7 @@
         <v>8.4852813742385695</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="2"/>
       <c r="B52" s="1" t="s">
         <v>59</v>
@@ -7720,7 +7750,7 @@
         <v>257.84389888162218</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="2"/>
       <c r="B53" s="1" t="s">
         <v>60</v>
@@ -7747,7 +7777,7 @@
         <v>2.994439290863427</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="2"/>
       <c r="B54" s="1" t="s">
         <v>62</v>
@@ -7774,7 +7804,7 @@
         <v>9.1233378824664317</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="2"/>
       <c r="B55" s="1" t="s">
         <v>64</v>
@@ -7801,7 +7831,7 @@
         <v>6.491019437140312</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="2"/>
       <c r="B56" s="1" t="s">
         <v>65</v>
@@ -7828,7 +7858,7 @@
         <v>2.368778400591983</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="2"/>
       <c r="B57" s="1" t="s">
         <v>66</v>
@@ -7855,7 +7885,7 @@
         <v>3.8658045015810671</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="2"/>
       <c r="B58" s="1" t="s">
         <v>70</v>
@@ -7882,7 +7912,7 @@
         <v>4.0604861645768864</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>88</v>
       </c>
@@ -7911,7 +7941,7 @@
         <v>4.7271206630739204</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="2"/>
       <c r="B60" s="1" t="s">
         <v>52</v>
@@ -7938,7 +7968,7 @@
         <v>125.3807698110984</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="2"/>
       <c r="B61" s="1" t="s">
         <v>55</v>
@@ -7965,7 +7995,7 @@
         <v>13.26272973410828</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="2"/>
       <c r="B62" s="1" t="s">
         <v>56</v>
@@ -7992,7 +8022,7 @@
         <v>117.21754536406431</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="2"/>
       <c r="B63" s="1" t="s">
         <v>57</v>
@@ -8019,7 +8049,7 @@
         <v>8.166132149660223</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="2"/>
       <c r="B64" s="1" t="s">
         <v>58</v>
@@ -8046,7 +8076,7 @@
         <v>206.27915771858989</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="2"/>
       <c r="B65" s="1" t="s">
         <v>59</v>
@@ -8073,7 +8103,7 @@
         <v>2.994439290863427</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="2"/>
       <c r="B66" s="1" t="s">
         <v>62</v>
@@ -8100,7 +8130,7 @@
         <v>2.6186146828319079</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="2"/>
       <c r="B67" s="1" t="s">
         <v>64</v>
@@ -8127,7 +8157,7 @@
         <v>3.7490511620121452</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="2"/>
       <c r="B68" s="1" t="s">
         <v>65</v>
@@ -8154,7 +8184,7 @@
         <v>5.8637303257681737</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="2"/>
       <c r="B69" s="1" t="s">
         <v>66</v>
@@ -8181,7 +8211,7 @@
         <v>13.4350288425444</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="2"/>
       <c r="B70" s="1" t="s">
         <v>70</v>
@@ -8208,7 +8238,7 @@
         <v>3.1561378461758052</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>89</v>
       </c>
@@ -8237,7 +8267,7 @@
         <v>5.7701762662738743</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="2"/>
       <c r="B72" s="1" t="s">
         <v>49</v>
@@ -8264,7 +8294,7 @@
         <v>123.0461392362734</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="2"/>
       <c r="B73" s="1" t="s">
         <v>50</v>
@@ -8291,7 +8321,7 @@
         <v>170.78469110047811</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="2"/>
       <c r="B74" s="1" t="s">
         <v>51</v>
@@ -8318,7 +8348,7 @@
         <v>43.441257545596642</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="2"/>
       <c r="B75" s="1" t="s">
         <v>53</v>
@@ -8345,7 +8375,7 @@
         <v>16.71227094083865</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="2"/>
       <c r="B76" s="1" t="s">
         <v>54</v>
@@ -8372,7 +8402,7 @@
         <v>6.2664070361617226</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="2"/>
       <c r="B77" s="1" t="s">
         <v>55</v>
@@ -8399,7 +8429,7 @@
         <v>2.3682757775922458</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="2"/>
       <c r="B78" s="1" t="s">
         <v>56</v>
@@ -8426,7 +8456,7 @@
         <v>284.76358615525271</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="2"/>
       <c r="B79" s="1" t="s">
         <v>57</v>
@@ -8453,7 +8483,7 @@
         <v>230.6519744839253</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="2"/>
       <c r="B80" s="1" t="s">
         <v>60</v>
@@ -8471,7 +8501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="2"/>
       <c r="B81" s="1" t="s">
         <v>61</v>
@@ -8498,7 +8528,7 @@
         <v>1.8708286933869711</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="2"/>
       <c r="B82" s="1" t="s">
         <v>62</v>
@@ -8525,7 +8555,7 @@
         <v>94.452810087012949</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="2"/>
       <c r="B83" s="1" t="s">
         <v>64</v>
@@ -8543,7 +8573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" s="2"/>
       <c r="B84" s="1" t="s">
         <v>67</v>
@@ -8561,7 +8591,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="2"/>
       <c r="B85" s="1" t="s">
         <v>68</v>
@@ -8588,7 +8618,7 @@
         <v>84.047785830623184</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="2"/>
       <c r="B86" s="1" t="s">
         <v>69</v>
@@ -8606,7 +8636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="2"/>
       <c r="B87" s="1" t="s">
         <v>70</v>
@@ -8633,7 +8663,7 @@
         <v>3.8369801240580421</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="2"/>
       <c r="B88" s="1" t="s">
         <v>71</v>
@@ -8660,7 +8690,7 @@
         <v>74.897151703741926</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>90</v>
       </c>
@@ -8689,7 +8719,7 @@
         <v>5.9046725125374211</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" s="2"/>
       <c r="B90" s="1" t="s">
         <v>52</v>
@@ -8716,7 +8746,7 @@
         <v>1.897366596101028</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" s="2"/>
       <c r="B91" s="1" t="s">
         <v>54</v>
@@ -8734,7 +8764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" s="2"/>
       <c r="B92" s="1" t="s">
         <v>55</v>
@@ -8761,7 +8791,7 @@
         <v>109.3943034913776</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" s="2"/>
       <c r="B93" s="1" t="s">
         <v>56</v>
@@ -8788,7 +8818,7 @@
         <v>197.5394194134989</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" s="2"/>
       <c r="B94" s="1" t="s">
         <v>57</v>
@@ -8815,7 +8845,7 @@
         <v>112.62737860436209</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" s="2"/>
       <c r="B95" s="1" t="s">
         <v>58</v>
@@ -8842,7 +8872,7 @@
         <v>3.6055512754639891</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" s="2"/>
       <c r="B96" s="1" t="s">
         <v>60</v>
@@ -8869,7 +8899,7 @@
         <v>181.49335931015281</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="2"/>
       <c r="B97" s="1" t="s">
         <v>62</v>
@@ -8896,7 +8926,7 @@
         <v>2.8084811086361499</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="2"/>
       <c r="B98" s="1" t="s">
         <v>64</v>
@@ -8923,7 +8953,7 @@
         <v>1.7728105208558369</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="2"/>
       <c r="B99" s="1" t="s">
         <v>65</v>
@@ -8950,7 +8980,7 @@
         <v>0.81649658092772615</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" s="2"/>
       <c r="B100" s="1" t="s">
         <v>66</v>
@@ -8977,7 +9007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" s="2"/>
       <c r="B101" s="1" t="s">
         <v>70</v>

</xml_diff>